<commit_message>
coding the fast tool function
</commit_message>
<xml_diff>
--- a/static/download/asset.xlsx
+++ b/static/download/asset.xlsx
@@ -54,14 +54,15 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>必填项</t>
+          <t>必填项
+在线:1
+离线：2</t>
         </r>
       </text>
     </comment>
@@ -129,12 +130,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="U2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+用户ID</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>管理IP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -228,7 +253,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>192.168.10.7</t>
+    <t>192.168.10.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.10.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.10.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有者ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -290,17 +327,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -324,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -332,7 +368,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -634,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -648,7 +683,7 @@
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -694,8 +729,11 @@
       <c r="T1">
         <v>19</v>
       </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -756,11 +794,17 @@
       <c r="T2" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="U2" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
@@ -771,7 +815,7 @@
         <v>22</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -779,11 +823,67 @@
       <c r="S3" s="3">
         <v>1</v>
       </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="S4" s="3">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="S5" s="3">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>